<commit_message>
Yard does not work on Excel
</commit_message>
<xml_diff>
--- a/Track_Resources/green_line_block_info.xlsx
+++ b/Track_Resources/green_line_block_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21722F60-3953-4B6F-A84C-495A6AF109A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CCE954-7AC1-49AE-9BEF-597F2DAFF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="62">
   <si>
     <t>Block Number</t>
   </si>
@@ -223,7 +223,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -606,11 +606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4415,7 +4415,7 @@
         <v>28</v>
       </c>
       <c r="I110" s="3">
-        <f t="shared" ref="I110:I151" si="10">E110*D110/100</f>
+        <f t="shared" ref="I110:I152" si="10">E110*D110/100</f>
         <v>0</v>
       </c>
       <c r="J110" s="3">
@@ -5635,7 +5635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5668,7 +5668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5701,7 +5701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5734,7 +5734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5767,7 +5767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5801,7 +5801,7 @@
         <v>33.119999999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5834,7 +5834,7 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -5867,15 +5867,114 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C152" s="3">
+        <v>0</v>
+      </c>
+      <c r="D152" s="3">
+        <v>0</v>
+      </c>
+      <c r="E152" s="3">
+        <v>0</v>
+      </c>
+      <c r="F152" s="3">
+        <v>0</v>
+      </c>
+      <c r="H152" s="3">
+        <v>0</v>
+      </c>
+      <c r="I152" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J152" s="1">
+        <v>0</v>
+      </c>
+      <c r="K152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="D153" s="3">
+        <v>0</v>
+      </c>
+      <c r="E153" s="3">
+        <v>0</v>
+      </c>
+      <c r="F153" s="3">
+        <v>0</v>
+      </c>
+      <c r="H153" s="3">
+        <v>0</v>
+      </c>
+      <c r="I153" s="1">
+        <f t="shared" ref="I153" si="14">E153*D153/100</f>
+        <v>0</v>
+      </c>
+      <c r="J153" s="1">
+        <v>0</v>
+      </c>
       <c r="K153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2</v>
+      </c>
+      <c r="D154" s="3">
+        <v>0</v>
+      </c>
+      <c r="E154" s="3">
+        <v>0</v>
+      </c>
+      <c r="F154" s="3">
+        <v>0</v>
+      </c>
+      <c r="H154" s="3">
+        <v>0</v>
+      </c>
+      <c r="I154" s="1">
+        <f t="shared" ref="I154" si="15">E154*D154/100</f>
+        <v>0</v>
+      </c>
+      <c r="J154" s="1">
+        <v>0</v>
+      </c>
+      <c r="K154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M157" s="1">
         <f>MIN(K2:K151)</f>
         <v>4.8461538461538467</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="K154" s="1">
-        <f>K153/1.2</f>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M158" s="1">
+        <f>M157/1.2</f>
         <v>4.0384615384615392</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes made from presentation
</commit_message>
<xml_diff>
--- a/Track_Resources/green_line_block_info.xlsx
+++ b/Track_Resources/green_line_block_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/lej40_pitt_edu/Documents/Documents/PITT - Spring 2024/ECE 1140 - Systems &amp; Project Engineering (TRAINS)/ECE-1140/Track_Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CCE954-7AC1-49AE-9BEF-597F2DAFF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A1CCE954-7AC1-49AE-9BEF-597F2DAFF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E98D98-CCA7-4798-9DEE-9A5BD619E3E0}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="62">
   <si>
     <t>Block Number</t>
   </si>
@@ -610,25 +610,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
     <col min="7" max="7" width="31" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" style="3"/>
-    <col min="9" max="12" width="8.81640625" style="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="8.796875" style="3"/>
+    <col min="9" max="12" width="8.796875" style="1"/>
+    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -663,7 +663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -683,22 +683,18 @@
         <v>45</v>
       </c>
       <c r="I2" s="3">
-        <f>E2*D2/100</f>
         <v>0.5</v>
       </c>
       <c r="J2" s="3">
-        <f>I2</f>
         <v>0.5</v>
       </c>
       <c r="K2" s="9">
-        <f t="shared" ref="K2:K65" si="0">D2*(1/(F2*1000/(60*60)))</f>
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="str">
-        <f>A2</f>
-        <v>Green</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -722,22 +718,18 @@
         <v>58</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I66" si="1">E3*D3/100</f>
         <v>1</v>
       </c>
       <c r="J3" s="3">
-        <f>I3+J2</f>
         <v>1.5</v>
       </c>
       <c r="K3" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="str">
-        <f t="shared" ref="A4:A70" si="2">A3</f>
-        <v>Green</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -755,23 +747,19 @@
         <v>45</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J67" si="3">I4+J3</f>
         <v>3</v>
       </c>
       <c r="K4" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -789,22 +777,18 @@
         <v>45</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K5" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -822,22 +806,18 @@
         <v>45</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -855,22 +835,18 @@
         <v>45</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="K7" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -889,22 +865,18 @@
       </c>
       <c r="G8" s="8"/>
       <c r="I8" s="3">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="K8" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -922,22 +894,18 @@
         <v>45</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="K9" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -961,22 +929,18 @@
         <v>58</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="K10" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -994,22 +958,18 @@
         <v>45</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
@@ -1027,22 +987,18 @@
         <v>45</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
       <c r="K12" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
@@ -1063,22 +1019,18 @@
         <v>50</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K13" s="9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
@@ -1096,22 +1048,18 @@
         <v>70</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K14" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7142857142857153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -1129,22 +1077,18 @@
         <v>70</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K15" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7142857142857153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>10</v>
@@ -1162,22 +1106,18 @@
         <v>70</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7142857142857153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
@@ -1201,22 +1141,18 @@
         <v>59</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K17" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7142857142857153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
@@ -1234,22 +1170,18 @@
         <v>60</v>
       </c>
       <c r="I18" s="3">
-        <f>E18*D18/100</f>
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
@@ -1267,22 +1199,18 @@
         <v>60</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1303,22 +1231,18 @@
         <v>49</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>11</v>
@@ -1336,22 +1260,18 @@
         <v>60</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -1369,22 +1289,18 @@
         <v>70</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="0"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>12</v>
@@ -1408,22 +1324,18 @@
         <v>59</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="0"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>12</v>
@@ -1441,22 +1353,18 @@
         <v>70</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="0"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A25" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>12</v>
@@ -1474,22 +1382,18 @@
         <v>70</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="0"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>12</v>
@@ -1507,22 +1411,18 @@
         <v>70</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" si="0"/>
-        <v>10.285714285714286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A27" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
@@ -1540,22 +1440,18 @@
         <v>70</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K27" s="9">
-        <f t="shared" si="0"/>
-        <v>5.1428571428571432</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>12</v>
@@ -1573,22 +1469,18 @@
         <v>30</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A29" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
@@ -1609,22 +1501,18 @@
         <v>61</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>13</v>
@@ -1642,22 +1530,18 @@
         <v>30</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A31" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
@@ -1675,22 +1559,18 @@
         <v>30</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1714,22 +1594,18 @@
         <v>58</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K32" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1747,22 +1623,18 @@
         <v>30</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K33" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A34" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>14</v>
@@ -1780,22 +1652,18 @@
         <v>30</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K34" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A35" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>14</v>
@@ -1813,22 +1681,18 @@
         <v>30</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K35" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>14</v>
@@ -1846,22 +1710,18 @@
         <v>30</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K36" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A37" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>15</v>
@@ -1882,22 +1742,18 @@
         <v>28</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K37" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="str">
-        <f>A34</f>
-        <v>Green</v>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A38" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>15</v>
@@ -1918,22 +1774,18 @@
         <v>28</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K38" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A39" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>15</v>
@@ -1954,22 +1806,18 @@
         <v>28</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J39" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>15</v>
@@ -1993,22 +1841,18 @@
         <v>60</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J40" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K40" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A41" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>15</v>
@@ -2029,22 +1873,18 @@
         <v>28</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J41" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K41" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>15</v>
@@ -2065,22 +1905,18 @@
         <v>28</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K42" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A43" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>15</v>
@@ -2101,22 +1937,18 @@
         <v>28</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K43" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A44" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
@@ -2137,22 +1969,18 @@
         <v>28</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K44" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A45" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>15</v>
@@ -2173,22 +2001,18 @@
         <v>28</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K45" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A46" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>15</v>
@@ -2209,22 +2033,18 @@
         <v>28</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A47" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>15</v>
@@ -2245,22 +2065,18 @@
         <v>28</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K47" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>15</v>
@@ -2281,22 +2097,18 @@
         <v>28</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K48" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A49" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>15</v>
@@ -2320,22 +2132,18 @@
         <v>60</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J49" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K49" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A50" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>15</v>
@@ -2356,22 +2164,18 @@
         <v>28</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K50" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A51" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>15</v>
@@ -2392,22 +2196,18 @@
         <v>28</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K51" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A52" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>15</v>
@@ -2428,22 +2228,18 @@
         <v>28</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J52" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K52" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A53" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>15</v>
@@ -2464,22 +2260,18 @@
         <v>28</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K53" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A54" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>15</v>
@@ -2500,22 +2292,18 @@
         <v>28</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J54" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K54" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A55" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>15</v>
@@ -2536,22 +2324,18 @@
         <v>28</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K55" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A56" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>15</v>
@@ -2572,22 +2356,18 @@
         <v>28</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J56" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K56" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A57" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>15</v>
@@ -2608,22 +2388,18 @@
         <v>28</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K57" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A58" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>15</v>
@@ -2647,22 +2423,18 @@
         <v>60</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J58" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K58" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A59" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>17</v>
@@ -2683,22 +2455,18 @@
         <v>51</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J59" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K59" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A60" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>17</v>
@@ -2716,22 +2484,18 @@
         <v>30</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K60" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A61" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>17</v>
@@ -2749,22 +2513,18 @@
         <v>30</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K61" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A62" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>17</v>
@@ -2782,22 +2542,18 @@
         <v>30</v>
       </c>
       <c r="I62" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J62" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K62" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A63" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>17</v>
@@ -2818,22 +2574,18 @@
         <v>52</v>
       </c>
       <c r="I63" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J63" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K63" s="9">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A64" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>18</v>
@@ -2851,22 +2603,18 @@
         <v>70</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K64" s="9">
-        <f t="shared" si="0"/>
-        <v>5.1428571428571432</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A65" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>18</v>
@@ -2884,22 +2632,18 @@
         <v>70</v>
       </c>
       <c r="I65" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J65" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K65" s="9">
-        <f t="shared" si="0"/>
-        <v>5.1428571428571432</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A66" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>18</v>
@@ -2923,22 +2667,18 @@
         <v>60</v>
       </c>
       <c r="I66" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J66" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K66" s="9">
-        <f t="shared" ref="K66:K129" si="4">D66*(1/(F66*1000/(60*60)))</f>
-        <v>10.285714285714286</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A67" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>18</v>
@@ -2956,22 +2696,18 @@
         <v>70</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" ref="I67:I77" si="5">E67*D67/100</f>
         <v>0</v>
       </c>
       <c r="J67" s="3">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K67" s="9">
-        <f t="shared" si="4"/>
-        <v>10.285714285714286</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A68" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>18</v>
@@ -2989,22 +2725,18 @@
         <v>40</v>
       </c>
       <c r="I68" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J68" s="3">
-        <f t="shared" ref="J68:J77" si="6">I68+J67</f>
         <v>0.5</v>
       </c>
       <c r="K68" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A69" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>18</v>
@@ -3022,22 +2754,18 @@
         <v>40</v>
       </c>
       <c r="I69" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J69" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K69" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Green</v>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A70" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>19</v>
@@ -3055,22 +2783,18 @@
         <v>40</v>
       </c>
       <c r="I70" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J70" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K70" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="str">
-        <f t="shared" ref="A71:A134" si="7">A70</f>
-        <v>Green</v>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A71" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>19</v>
@@ -3088,22 +2812,18 @@
         <v>40</v>
       </c>
       <c r="I71" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J71" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K71" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A72" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>19</v>
@@ -3121,22 +2841,18 @@
         <v>40</v>
       </c>
       <c r="I72" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J72" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K72" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A73" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>19</v>
@@ -3154,22 +2870,18 @@
         <v>40</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J73" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K73" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A74" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>19</v>
@@ -3193,22 +2905,18 @@
         <v>60</v>
       </c>
       <c r="I74" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J74" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K74" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A75" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>20</v>
@@ -3226,22 +2934,18 @@
         <v>40</v>
       </c>
       <c r="I75" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J75" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K75" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A76" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>20</v>
@@ -3259,22 +2963,18 @@
         <v>40</v>
       </c>
       <c r="I76" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J76" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K76" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A77" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>20</v>
@@ -3295,22 +2995,18 @@
         <v>53</v>
       </c>
       <c r="I77" s="3">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J77" s="3">
-        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K77" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A78" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>21</v>
@@ -3334,22 +3030,18 @@
         <v>59</v>
       </c>
       <c r="I78" s="3">
-        <f t="shared" ref="I78:I109" si="8">E78*D78/100</f>
         <v>0</v>
       </c>
       <c r="J78" s="3">
-        <f t="shared" ref="J78:J109" si="9">I78+J77</f>
         <v>0.5</v>
       </c>
       <c r="K78" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A79" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>21</v>
@@ -3367,22 +3059,18 @@
         <v>70</v>
       </c>
       <c r="I79" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J79" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K79" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A80" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>21</v>
@@ -3400,22 +3088,18 @@
         <v>70</v>
       </c>
       <c r="I80" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J80" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K80" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A81" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>21</v>
@@ -3433,22 +3117,18 @@
         <v>70</v>
       </c>
       <c r="I81" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J81" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K81" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A82" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>21</v>
@@ -3466,22 +3146,18 @@
         <v>70</v>
       </c>
       <c r="I82" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J82" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K82" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A83" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A83" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>21</v>
@@ -3499,22 +3175,18 @@
         <v>70</v>
       </c>
       <c r="I83" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J83" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K83" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A84" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>21</v>
@@ -3532,22 +3204,18 @@
         <v>70</v>
       </c>
       <c r="I84" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J84" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K84" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A85" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>21</v>
@@ -3565,22 +3233,18 @@
         <v>70</v>
       </c>
       <c r="I85" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J85" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K85" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A86" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>21</v>
@@ -3601,22 +3265,18 @@
         <v>55</v>
       </c>
       <c r="I86" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J86" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K86" s="9">
-        <f t="shared" si="4"/>
-        <v>15.428571428571431</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A87" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A87" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>22</v>
@@ -3634,22 +3294,18 @@
         <v>25</v>
       </c>
       <c r="I87" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J87" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K87" s="9">
-        <f t="shared" si="4"/>
-        <v>14.399999999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A88" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>22</v>
@@ -3667,22 +3323,18 @@
         <v>25</v>
       </c>
       <c r="I88" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J88" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K88" s="9">
-        <f t="shared" si="4"/>
-        <v>12.470399999999998</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A89" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>22</v>
@@ -3706,22 +3358,18 @@
         <v>58</v>
       </c>
       <c r="I89" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J89" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K89" s="9">
-        <f t="shared" si="4"/>
-        <v>14.399999999999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A90" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>23</v>
@@ -3739,22 +3387,18 @@
         <v>25</v>
       </c>
       <c r="I90" s="3">
-        <f t="shared" si="8"/>
         <v>-0.375</v>
       </c>
       <c r="J90" s="3">
-        <f t="shared" si="9"/>
         <v>0.125</v>
       </c>
       <c r="K90" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A91" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>23</v>
@@ -3772,22 +3416,18 @@
         <v>25</v>
       </c>
       <c r="I91" s="3">
-        <f t="shared" si="8"/>
         <v>-0.75</v>
       </c>
       <c r="J91" s="3">
-        <f t="shared" si="9"/>
         <v>-0.625</v>
       </c>
       <c r="K91" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A92" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>23</v>
@@ -3805,22 +3445,18 @@
         <v>25</v>
       </c>
       <c r="I92" s="3">
-        <f t="shared" si="8"/>
         <v>-1.5</v>
       </c>
       <c r="J92" s="3">
-        <f t="shared" si="9"/>
         <v>-2.125</v>
       </c>
       <c r="K92" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A93" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>23</v>
@@ -3838,22 +3474,18 @@
         <v>25</v>
       </c>
       <c r="I93" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J93" s="3">
-        <f t="shared" si="9"/>
         <v>-2.125</v>
       </c>
       <c r="K93" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A94" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>23</v>
@@ -3871,22 +3503,18 @@
         <v>25</v>
       </c>
       <c r="I94" s="3">
-        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
       <c r="J94" s="3">
-        <f t="shared" si="9"/>
         <v>-0.625</v>
       </c>
       <c r="K94" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A95" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>23</v>
@@ -3904,22 +3532,18 @@
         <v>25</v>
       </c>
       <c r="I95" s="3">
-        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
       <c r="J95" s="3">
-        <f t="shared" si="9"/>
         <v>0.125</v>
       </c>
       <c r="K95" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A96" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>23</v>
@@ -3937,22 +3561,18 @@
         <v>25</v>
       </c>
       <c r="I96" s="3">
-        <f t="shared" si="8"/>
         <v>0.375</v>
       </c>
       <c r="J96" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K96" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A97" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>23</v>
@@ -3976,22 +3596,18 @@
         <v>58</v>
       </c>
       <c r="I97" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J97" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K97" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A98" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>23</v>
@@ -4009,22 +3625,18 @@
         <v>25</v>
       </c>
       <c r="I98" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J98" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K98" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A99" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>24</v>
@@ -4042,22 +3654,18 @@
         <v>25</v>
       </c>
       <c r="I99" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J99" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K99" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A100" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>24</v>
@@ -4075,22 +3683,18 @@
         <v>25</v>
       </c>
       <c r="I100" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J100" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K100" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A101" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>24</v>
@@ -4108,22 +3712,18 @@
         <v>25</v>
       </c>
       <c r="I101" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J101" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K101" s="9">
-        <f t="shared" si="4"/>
-        <v>10.799999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A102" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>25</v>
@@ -4141,22 +3741,18 @@
         <v>26</v>
       </c>
       <c r="I102" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J102" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K102" s="9">
-        <f t="shared" si="4"/>
-        <v>4.8461538461538467</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A103" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>26</v>
@@ -4174,22 +3770,18 @@
         <v>28</v>
       </c>
       <c r="I103" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J103" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K103" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A104" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>26</v>
@@ -4207,22 +3799,18 @@
         <v>28</v>
       </c>
       <c r="I104" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J104" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K104" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A105" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>26</v>
@@ -4240,22 +3828,18 @@
         <v>28</v>
       </c>
       <c r="I105" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J105" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K105" s="9">
-        <f t="shared" si="4"/>
-        <v>10.285714285714286</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A106" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A106" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>27</v>
@@ -4272,30 +3856,25 @@
       <c r="F106" s="3">
         <v>28</v>
       </c>
-      <c r="G106" s="8" t="str">
-        <f>G74</f>
-        <v>STATION; DORMONT</v>
+      <c r="G106" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>60</v>
       </c>
       <c r="I106" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J106" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K106" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A107" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A107" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>27</v>
@@ -4313,22 +3892,18 @@
         <v>28</v>
       </c>
       <c r="I107" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J107" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K107" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A108" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>27</v>
@@ -4346,22 +3921,18 @@
         <v>28</v>
       </c>
       <c r="I108" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J108" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K108" s="9">
-        <f t="shared" si="4"/>
-        <v>11.571428571428573</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A109" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A109" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>27</v>
@@ -4382,22 +3953,18 @@
         <v>49</v>
       </c>
       <c r="I109" s="3">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J109" s="3">
-        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="K109" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A110" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>27</v>
@@ -4415,22 +3982,18 @@
         <v>28</v>
       </c>
       <c r="I110" s="3">
-        <f t="shared" ref="I110:I152" si="10">E110*D110/100</f>
         <v>0</v>
       </c>
       <c r="J110" s="3">
-        <f t="shared" ref="J110:J151" si="11">I110+J109</f>
         <v>0.5</v>
       </c>
       <c r="K110" s="9">
-        <f t="shared" si="4"/>
-        <v>12.857142857142859</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A111" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>32</v>
@@ -4448,22 +4011,18 @@
         <v>30</v>
       </c>
       <c r="I111" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J111" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K111" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A112" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>32</v>
@@ -4481,22 +4040,18 @@
         <v>30</v>
       </c>
       <c r="I112" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J112" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K112" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A113" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>32</v>
@@ -4514,22 +4069,18 @@
         <v>30</v>
       </c>
       <c r="I113" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J113" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K113" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A114" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>32</v>
@@ -4547,22 +4098,18 @@
         <v>30</v>
       </c>
       <c r="I114" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J114" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K114" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A115" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>32</v>
@@ -4571,7 +4118,6 @@
         <v>114</v>
       </c>
       <c r="D115" s="3">
-        <f>100+62</f>
         <v>162</v>
       </c>
       <c r="E115" s="3">
@@ -4580,30 +4126,25 @@
       <c r="F115" s="3">
         <v>30</v>
       </c>
-      <c r="G115" s="8" t="str">
-        <f>G66</f>
-        <v>STATION; GLENBURY</v>
+      <c r="G115" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>60</v>
       </c>
       <c r="I115" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J115" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K115" s="9">
-        <f t="shared" si="4"/>
-        <v>19.439999999999998</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A116" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A116" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>32</v>
@@ -4621,22 +4162,18 @@
         <v>30</v>
       </c>
       <c r="I116" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J116" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K116" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A117" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>32</v>
@@ -4654,22 +4191,18 @@
         <v>30</v>
       </c>
       <c r="I117" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J117" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K117" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A118" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>33</v>
@@ -4687,22 +4220,18 @@
         <v>15</v>
       </c>
       <c r="I118" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J118" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K118" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A119" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>33</v>
@@ -4720,22 +4249,18 @@
         <v>15</v>
       </c>
       <c r="I119" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J119" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K119" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A120" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>33</v>
@@ -4753,22 +4278,18 @@
         <v>15</v>
       </c>
       <c r="I120" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J120" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K120" s="9">
-        <f t="shared" si="4"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A121" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>33</v>
@@ -4786,22 +4307,18 @@
         <v>15</v>
       </c>
       <c r="I121" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J121" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K121" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A122" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A122" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>33</v>
@@ -4819,22 +4336,18 @@
         <v>15</v>
       </c>
       <c r="I122" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J122" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K122" s="9">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A123" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>34</v>
@@ -4855,22 +4368,18 @@
         <v>28</v>
       </c>
       <c r="I123" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J123" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K123" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A124" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>34</v>
@@ -4887,30 +4396,25 @@
       <c r="F124" s="3">
         <v>20</v>
       </c>
-      <c r="G124" s="8" t="str">
-        <f>G58</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
+      <c r="G124" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>60</v>
       </c>
       <c r="I124" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J124" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K124" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A125" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A125" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>34</v>
@@ -4931,22 +4435,18 @@
         <v>28</v>
       </c>
       <c r="I125" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J125" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K125" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A126" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A126" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>34</v>
@@ -4967,22 +4467,18 @@
         <v>28</v>
       </c>
       <c r="I126" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J126" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K126" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A127" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>34</v>
@@ -5003,22 +4499,18 @@
         <v>28</v>
       </c>
       <c r="I127" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J127" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K127" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A128" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A128" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>34</v>
@@ -5039,22 +4531,18 @@
         <v>28</v>
       </c>
       <c r="I128" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J128" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K128" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A129" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>34</v>
@@ -5075,22 +4563,18 @@
         <v>28</v>
       </c>
       <c r="I129" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J129" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K129" s="9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A130" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>34</v>
@@ -5111,22 +4595,18 @@
         <v>28</v>
       </c>
       <c r="I130" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J130" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K130" s="9">
-        <f t="shared" ref="K130:K150" si="12">D130*(1/(F130*1000/(60*60)))</f>
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A131" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>34</v>
@@ -5147,22 +4627,18 @@
         <v>28</v>
       </c>
       <c r="I131" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J131" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K131" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A132" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>34</v>
@@ -5183,22 +4659,18 @@
         <v>28</v>
       </c>
       <c r="I132" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J132" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K132" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A133" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A133" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>34</v>
@@ -5215,30 +4687,25 @@
       <c r="F133" s="3">
         <v>20</v>
       </c>
-      <c r="G133" s="8" t="str">
-        <f>G49</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      <c r="G133" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="H133" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I133" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J133" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K133" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>Green</v>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A134" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>34</v>
@@ -5259,22 +4726,18 @@
         <v>28</v>
       </c>
       <c r="I134" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J134" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K134" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="str">
-        <f t="shared" ref="A135:A151" si="13">A134</f>
-        <v>Green</v>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A135" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>34</v>
@@ -5295,22 +4758,18 @@
         <v>28</v>
       </c>
       <c r="I135" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J135" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K135" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A136" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>34</v>
@@ -5331,22 +4790,18 @@
         <v>28</v>
       </c>
       <c r="I136" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J136" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K136" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A137" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A137" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>34</v>
@@ -5367,22 +4822,18 @@
         <v>28</v>
       </c>
       <c r="I137" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J137" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K137" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A138" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A138" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>34</v>
@@ -5403,22 +4854,18 @@
         <v>28</v>
       </c>
       <c r="I138" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J138" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K138" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A139" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>34</v>
@@ -5439,22 +4886,18 @@
         <v>28</v>
       </c>
       <c r="I139" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J139" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K139" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A140" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A140" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>34</v>
@@ -5475,22 +4918,18 @@
         <v>28</v>
       </c>
       <c r="I140" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J140" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K140" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A141" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A141" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>34</v>
@@ -5511,22 +4950,18 @@
         <v>28</v>
       </c>
       <c r="I141" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J141" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K141" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A142" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A142" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>34</v>
@@ -5543,30 +4978,25 @@
       <c r="F142" s="3">
         <v>20</v>
       </c>
-      <c r="G142" s="8" t="str">
-        <f>G40</f>
-        <v>STATION; CENTRAL; UNDERDROUND</v>
+      <c r="G142" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>60</v>
       </c>
       <c r="I142" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J142" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K142" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A143" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>34</v>
@@ -5587,22 +5017,18 @@
         <v>28</v>
       </c>
       <c r="I143" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J143" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K143" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A144" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A144" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>34</v>
@@ -5623,22 +5049,18 @@
         <v>28</v>
       </c>
       <c r="I144" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J144" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K144" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A145" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>35</v>
@@ -5656,22 +5078,18 @@
         <v>20</v>
       </c>
       <c r="I145" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J145" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K145" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A146" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A146" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>35</v>
@@ -5689,22 +5107,18 @@
         <v>20</v>
       </c>
       <c r="I146" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J146" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K146" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A147" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>35</v>
@@ -5722,22 +5136,18 @@
         <v>20</v>
       </c>
       <c r="I147" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J147" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K147" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A148" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>36</v>
@@ -5755,22 +5165,18 @@
         <v>20</v>
       </c>
       <c r="I148" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J148" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K148" s="9">
-        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A149" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>36</v>
@@ -5779,7 +5185,6 @@
         <v>148</v>
       </c>
       <c r="D149" s="3">
-        <f>40+144</f>
         <v>184</v>
       </c>
       <c r="E149" s="3">
@@ -5789,22 +5194,18 @@
         <v>20</v>
       </c>
       <c r="I149" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J149" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K149" s="9">
-        <f t="shared" si="12"/>
-        <v>33.119999999999997</v>
-      </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A150" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A150" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>36</v>
@@ -5822,22 +5223,18 @@
         <v>20</v>
       </c>
       <c r="I150" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J150" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K150" s="9">
-        <f t="shared" si="12"/>
-        <v>7.1999999999999993</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A151" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Green</v>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A151" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>37</v>
@@ -5855,19 +5252,16 @@
         <v>20</v>
       </c>
       <c r="I151" s="3">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J151" s="3">
-        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="K151" s="9">
-        <f>D151*(1/(F151*1000/(60*60)))</f>
         <v>6.3</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A152" s="3" t="s">
         <v>2</v>
       </c>
@@ -5890,7 +5284,7 @@
         <v>0</v>
       </c>
       <c r="I152" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="I110:I152" si="0">E152*D152/100</f>
         <v>0</v>
       </c>
       <c r="J152" s="1">
@@ -5900,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A153" s="3" t="s">
         <v>2</v>
       </c>
@@ -5923,7 +5317,7 @@
         <v>0</v>
       </c>
       <c r="I153" s="1">
-        <f t="shared" ref="I153" si="14">E153*D153/100</f>
+        <f t="shared" ref="I153" si="1">E153*D153/100</f>
         <v>0</v>
       </c>
       <c r="J153" s="1">
@@ -5933,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A154" s="3" t="s">
         <v>2</v>
       </c>
@@ -5956,7 +5350,7 @@
         <v>0</v>
       </c>
       <c r="I154" s="1">
-        <f t="shared" ref="I154" si="15">E154*D154/100</f>
+        <f t="shared" ref="I154" si="2">E154*D154/100</f>
         <v>0</v>
       </c>
       <c r="J154" s="1">
@@ -5966,16 +5360,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.5">
       <c r="M157" s="1">
         <f>MIN(K2:K151)</f>
-        <v>4.8461538461538467</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.5">
       <c r="M158" s="1">
         <f>M157/1.2</f>
-        <v>4.0384615384615392</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing grade to train model
</commit_message>
<xml_diff>
--- a/Track_Resources/green_line_block_info.xlsx
+++ b/Track_Resources/green_line_block_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/lej40_pitt_edu/Documents/Documents/PITT - Spring 2024/ECE 1140 - Systems &amp; Project Engineering (TRAINS)/ECE-1140/Track_Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A1CCE954-7AC1-49AE-9BEF-597F2DAFF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E98D98-CCA7-4798-9DEE-9A5BD619E3E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D252C6-93C7-49A6-B400-0A704C34B58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -609,26 +609,26 @@
   <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="3"/>
-    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
     <col min="7" max="7" width="31" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" style="3"/>
-    <col min="9" max="12" width="8.796875" style="1"/>
-    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.796875" style="1"/>
+    <col min="8" max="8" width="8.81640625" style="3"/>
+    <col min="9" max="12" width="8.81640625" style="1"/>
+    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -663,7 +663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -692,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -727,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -757,7 +757,7 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -786,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -815,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -844,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -903,7 +903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -938,7 +938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -967,7 +967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -996,7 +996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>2</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>2</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>100</v>
       </c>
       <c r="E70" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F70" s="3">
         <v>40</v>
@@ -2792,7 +2792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>2</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>100</v>
       </c>
       <c r="E71" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F71" s="3">
         <v>40</v>
@@ -2821,7 +2821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>2</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>100</v>
       </c>
       <c r="E72" s="3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F72" s="3">
         <v>40</v>
@@ -2850,7 +2850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>2</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>100</v>
       </c>
       <c r="E73" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F73" s="3">
         <v>40</v>
@@ -2879,7 +2879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>2</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>100</v>
       </c>
       <c r="E74" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F74" s="3">
         <v>40</v>
@@ -2914,7 +2914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>2</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>100</v>
       </c>
       <c r="E75" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F75" s="3">
         <v>40</v>
@@ -2943,7 +2943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>2</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>100</v>
       </c>
       <c r="E76" s="3">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F76" s="3">
         <v>40</v>
@@ -2972,7 +2972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>2</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>100</v>
       </c>
       <c r="E77" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F77" s="3">
         <v>40</v>
@@ -3004,7 +3004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>2</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>300</v>
       </c>
       <c r="E78" s="3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F78" s="3">
         <v>70</v>
@@ -3039,7 +3039,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>300</v>
       </c>
       <c r="E79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="3">
         <v>70</v>
@@ -3068,7 +3068,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>2</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>300</v>
       </c>
       <c r="E80" s="3">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F80" s="3">
         <v>70</v>
@@ -3097,7 +3097,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>2</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>300</v>
       </c>
       <c r="E81" s="3">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F81" s="3">
         <v>70</v>
@@ -3126,7 +3126,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>2</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>2</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>2</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>2</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>2</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>2</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>2</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>2</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>2</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>2</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>2</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>2</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>2</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>2</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>2</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>2</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>2</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>2</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>2</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>2</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>2</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>2</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>2</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>2</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>2</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>2</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>2</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>2</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>2</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>2</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>2</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>2</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>2</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>2</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>2</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>2</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>2</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>2</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>2</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>2</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>2</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>2</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>2</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>2</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>2</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>2</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>2</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>2</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>2</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>2</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>2</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>2</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>2</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>2</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>2</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>2</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>2</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>2</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>2</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>2</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>2</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>2</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>2</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>2</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>2</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>2</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>0</v>
       </c>
       <c r="I152" s="1">
-        <f t="shared" ref="I110:I152" si="0">E152*D152/100</f>
+        <f t="shared" ref="I152" si="0">E152*D152/100</f>
         <v>0</v>
       </c>
       <c r="J152" s="1">
@@ -5294,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
         <v>2</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>2</v>
       </c>
@@ -5360,13 +5360,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M157" s="1">
         <f>MIN(K2:K151)</f>
         <v>4.8</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M158" s="1">
         <f>M157/1.2</f>
         <v>4</v>

</xml_diff>

<commit_message>
switch block figured out
</commit_message>
<xml_diff>
--- a/Track_Resources/green_line_block_info.xlsx
+++ b/Track_Resources/green_line_block_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D252C6-93C7-49A6-B400-0A704C34B58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBD75E7-C4E9-4975-B7C2-6D1458376F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
   <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2777,7 +2777,7 @@
         <v>100</v>
       </c>
       <c r="E70" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="3">
         <v>40</v>
@@ -2806,7 +2806,7 @@
         <v>100</v>
       </c>
       <c r="E71" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F71" s="3">
         <v>40</v>
@@ -2835,7 +2835,7 @@
         <v>100</v>
       </c>
       <c r="E72" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F72" s="3">
         <v>40</v>
@@ -2864,7 +2864,7 @@
         <v>100</v>
       </c>
       <c r="E73" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F73" s="3">
         <v>40</v>
@@ -2893,7 +2893,7 @@
         <v>100</v>
       </c>
       <c r="E74" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F74" s="3">
         <v>40</v>
@@ -2928,7 +2928,7 @@
         <v>100</v>
       </c>
       <c r="E75" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F75" s="3">
         <v>40</v>
@@ -2957,7 +2957,7 @@
         <v>100</v>
       </c>
       <c r="E76" s="3">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F76" s="3">
         <v>40</v>
@@ -2986,7 +2986,7 @@
         <v>100</v>
       </c>
       <c r="E77" s="3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F77" s="3">
         <v>40</v>
@@ -3018,7 +3018,7 @@
         <v>300</v>
       </c>
       <c r="E78" s="3">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F78" s="3">
         <v>70</v>
@@ -3053,7 +3053,7 @@
         <v>300</v>
       </c>
       <c r="E79" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" s="3">
         <v>70</v>
@@ -3082,7 +3082,7 @@
         <v>300</v>
       </c>
       <c r="E80" s="3">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F80" s="3">
         <v>70</v>
@@ -3111,7 +3111,7 @@
         <v>300</v>
       </c>
       <c r="E81" s="3">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F81" s="3">
         <v>70</v>

</xml_diff>